<commit_message>
Minor changes and link revision
</commit_message>
<xml_diff>
--- a/FundingCleanedFinal.xlsx
+++ b/FundingCleanedFinal.xlsx
@@ -16427,8 +16427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2074"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18143,7 +18143,7 @@
         <v>5297</v>
       </c>
       <c r="I59">
-        <v>3900000000</v>
+        <v>54000000</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>